<commit_message>
Tried to add LS
</commit_message>
<xml_diff>
--- a/GrizWt.xlsx
+++ b/GrizWt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/massey/Dropbox/Griz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F363228B-CD6E-6044-A9D7-C54BFBAAA2B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6B7A90-A0C9-3147-ADFA-59BE804EC5B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="28260" windowHeight="16220" xr2:uid="{442F6D33-47C8-EF45-9E8B-4B6E9BCB0EB8}"/>
   </bookViews>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DF0AEF-0FAE-B446-938E-395ABA109CC9}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -583,6 +583,30 @@
         <v>44551</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>8.9</v>
+      </c>
+      <c r="B25" s="1">
+        <v>44552</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>7.4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44556</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>11.1</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44557</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Went to 2nd order
</commit_message>
<xml_diff>
--- a/GrizWt.xlsx
+++ b/GrizWt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/massey/Dropbox/Griz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F88BCDC-14BD-BE4E-83A7-AC37986A09FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C521EF-2450-2748-8599-B048384C17E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="460" windowWidth="28260" windowHeight="16220" xr2:uid="{442F6D33-47C8-EF45-9E8B-4B6E9BCB0EB8}"/>
   </bookViews>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DF0AEF-0FAE-B446-938E-395ABA109CC9}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -437,7 +437,7 @@
         <v>44525</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C30" si="0">B4-$B$2</f>
+        <f t="shared" ref="C4:C37" si="0">B4-$B$2</f>
         <v>3</v>
       </c>
     </row>
@@ -751,6 +751,90 @@
       <c r="C30">
         <f t="shared" si="0"/>
         <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>5.6</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44561</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>6.1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44562</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>7.5</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44563</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>8.9</v>
+      </c>
+      <c r="B34" s="1">
+        <v>44565</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>8.4</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44566</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44570</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>4.5</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44572</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>